<commit_message>
change filename + fenetre saccade
</commit_message>
<xml_diff>
--- a/m n° 001.xlsx
+++ b/m n° 001.xlsx
@@ -572,19 +572,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" t="n">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" t="n">
-        <v>51.72835159301758</v>
+        <v>52.30021667480469</v>
       </c>
       <c r="E5" t="n">
-        <v>66.40760803222656</v>
+        <v>66.3616943359375</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3400270044803619</v>
+        <v>0.3898895084857941</v>
       </c>
       <c r="G5" t="n">
         <v>0.3400270044803619</v>
@@ -601,13 +601,13 @@
         <v>71</v>
       </c>
       <c r="D6" t="n">
-        <v>56.54074478149414</v>
+        <v>56.42783355712891</v>
       </c>
       <c r="E6" t="n">
-        <v>66.78765869140625</v>
+        <v>66.79560089111328</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7279419898986816</v>
+        <v>0.7200009822845459</v>
       </c>
       <c r="G6" t="n">
         <v>0.7279419898986816</v>
@@ -813,19 +813,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-86</v>
+        <v>-87</v>
       </c>
       <c r="C3" t="n">
         <v>-60</v>
       </c>
       <c r="D3" t="n">
-        <v>54.27056503295898</v>
+        <v>54.81571960449219</v>
       </c>
       <c r="E3" t="n">
-        <v>53.4715461730957</v>
+        <v>53.42763900756836</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5408340096473694</v>
+        <v>0.5847430229187012</v>
       </c>
       <c r="G3" t="n">
         <v>0.5408340096473694</v>
@@ -928,19 +928,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>53.7308349609375</v>
+        <v>54.98033142089844</v>
       </c>
       <c r="E8" t="n">
-        <v>57.57965469360352</v>
+        <v>57.45763778686523</v>
       </c>
       <c r="F8" t="n">
-        <v>0.503958523273468</v>
+        <v>0.6259744763374329</v>
       </c>
       <c r="G8" t="n">
         <v>0.5000219941139221</v>

</xml_diff>